<commit_message>
Hide first row and col on ID Server tab in setupdata xls
</commit_message>
<xml_diff>
--- a/bika/lims/setupdata/test/test.xlsx
+++ b/bika/lims/setupdata/test/test.xlsx
@@ -6133,7 +6133,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="98.1214574898785"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="98.9797570850202"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -6203,8 +6203,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -6254,8 +6254,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -6356,8 +6356,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2105263157895"/>
     <col collapsed="false" hidden="false" max="5" min="3" style="0" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -6696,14 +6696,14 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.21052631578947"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.53441295546559"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.85425101214575"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.6720647773279"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.85425101214575"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.96356275303644"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.60728744939271"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="24.6356275303644"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="24.8502024291498"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.31983805668016"/>
   </cols>
   <sheetData>
@@ -6881,10 +6881,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6396761133603"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="40" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="40" width="12.1052631578947"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="40" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="40" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="40" width="12.5344129554656"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -7060,12 +7060,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.2429149797571"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.74898785425101"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.6761133603239"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -7286,8 +7286,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -7397,13 +7397,13 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.5668016194332"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.74898785425101"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.49797570850202"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.74898785425101"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.60728744939271"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.4615384615385"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.5668016194332"/>
     <col collapsed="false" hidden="false" max="1023" min="9" style="0" width="6.74898785425101"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="5.78542510121457"/>
   </cols>
@@ -7782,7 +7782,7 @@
   </sheetData>
   <dataValidations count="6">
     <dataValidation allowBlank="false" error="Select 0 or 1  from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 1 (True) or 0 (False) from the drop-down menu" promptTitle="Does the client get membership discount?" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4:D8 D10:D14" type="list">
-      <formula1>Constants!$G$2:$G$3</formula1>
+      <formula1>constaa s!$g$2:ug$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" prompt="Enter a number and recognised unit separated by a space, e.g. 100 g or 50 ml" promptTitle="Entry format:" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="G4:G15" type="none">
@@ -7833,10 +7833,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.9230769230769"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.0323886639676"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1018" min="9" style="0" width="8.57085020242915"/>
@@ -8128,9 +8128,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.0647773279352"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2834008097166"/>
     <col collapsed="false" hidden="false" max="1018" min="4" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1019" style="0" width="5.1417004048583"/>
   </cols>
@@ -8196,24 +8196,24 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="20.1376518218623"/>
+    <col collapsed="false" hidden="true" max="1" min="1" style="5" width="0"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="20.246963562753"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="5" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="5" width="6.21457489878543"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="7.39271255060729"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="7.49797570850202"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="9.85425101214575"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="true" ht="12.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="6" customFormat="true" ht="12.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
@@ -8316,6 +8316,7 @@
         <v>34</v>
       </c>
       <c r="E5" s="10"/>
+      <c r="F5" s="0"/>
       <c r="G5" s="0"/>
       <c r="H5" s="5" t="s">
         <v>35</v>
@@ -8338,6 +8339,7 @@
         <v>34</v>
       </c>
       <c r="E6" s="10"/>
+      <c r="F6" s="0"/>
       <c r="G6" s="0"/>
       <c r="H6" s="5" t="s">
         <v>29</v>
@@ -8360,6 +8362,7 @@
         <v>34</v>
       </c>
       <c r="E7" s="10"/>
+      <c r="F7" s="0"/>
       <c r="G7" s="0"/>
       <c r="H7" s="5" t="s">
         <v>40</v>
@@ -8382,6 +8385,7 @@
         <v>34</v>
       </c>
       <c r="E8" s="10"/>
+      <c r="F8" s="0"/>
       <c r="G8" s="0"/>
       <c r="H8" s="5" t="s">
         <v>43</v>
@@ -8404,6 +8408,7 @@
         <v>34</v>
       </c>
       <c r="E9" s="10"/>
+      <c r="F9" s="0"/>
       <c r="G9" s="0"/>
       <c r="H9" s="5" t="s">
         <v>47</v>
@@ -8426,6 +8431,7 @@
         <v>34</v>
       </c>
       <c r="E10" s="10"/>
+      <c r="F10" s="0"/>
       <c r="G10" s="0"/>
       <c r="H10" s="5" t="s">
         <v>51</v>
@@ -8448,6 +8454,7 @@
         <v>34</v>
       </c>
       <c r="E11" s="10"/>
+      <c r="F11" s="0"/>
       <c r="G11" s="0"/>
       <c r="H11" s="5" t="s">
         <v>55</v>
@@ -8470,6 +8477,7 @@
         <v>34</v>
       </c>
       <c r="E12" s="10"/>
+      <c r="F12" s="0"/>
       <c r="G12" s="0"/>
       <c r="H12" s="5" t="s">
         <v>59</v>
@@ -8550,11 +8558,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="57.417004048583"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="86" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="57.9514170040486"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="86" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.1376518218623"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -8811,8 +8819,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -8953,9 +8961,9 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="9.85425101214575"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="21" min="6" style="0" width="9.85425101214575"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="21" min="6" style="0" width="9.96356275303644"/>
     <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -9183,7 +9191,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="21" min="2" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.57085020242915"/>
   </cols>
@@ -9462,8 +9470,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.3522267206478"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="7.71255060728745"/>
   </cols>
   <sheetData>
@@ -9582,26 +9590,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.6761133603239"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.4615384615385"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.4574898785425"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="21.8542510121457"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.9959514170041"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="22.0647773279352"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.8178137651822"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.7813765182186"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.8906882591093"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="22.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -10753,18 +10761,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0647773279352"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.6761133603239"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="34.17004048583"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="32.9919028340081"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="39.3117408906883"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="34.4939271255061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="33.2064777327935"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="39.6356275303644"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="7.71255060728745"/>
   </cols>
   <sheetData>
@@ -10944,17 +10952,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.8866396761134"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.7813765182186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0323886639676"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.85425101214575"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.9230769230769"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.9595141700405"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.4574898785425"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.2064777327935"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.8866396761134"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="36.2064777327935"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.1740890688259"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.6720647773279"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="36.5263157894737"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="7.71255060728745"/>
   </cols>
   <sheetData>
@@ -11127,11 +11135,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.6761133603239"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5708502024291"/>
   </cols>
@@ -11265,15 +11273,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.6396761133603"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.3522267206478"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.3157894736842"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.5303643724696"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="7.71255060728745"/>
   </cols>
@@ -12135,8 +12143,8 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.7408906882591"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.0647773279352"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8906882591093"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.74898785425101"/>
   </cols>
   <sheetData>
@@ -12537,15 +12545,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.4615384615385"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.6356275303644"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6396761133603"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.71255060728745"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.6761133603239"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.7449392712551"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="5.35627530364372"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="7.71255060728745"/>
   </cols>
@@ -12764,15 +12772,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.7813765182186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.246963562753"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.7813765182186"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.71255060728745"/>
   </cols>
   <sheetData>
@@ -12866,9 +12874,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2064777327935"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.5263157894737"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="21.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -12969,9 +12977,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.7732793522267"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.2024291497976"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.8461538461539"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.31983805668016"/>
   </cols>
   <sheetData>
@@ -13107,8 +13115,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="7.39271255060729"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="3.31983805668016"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
@@ -13715,13 +13723,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="29.9919028340081"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.35627530364372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.71255060728745"/>
@@ -13734,7 +13741,7 @@
     <col collapsed="false" hidden="false" max="20" min="20" style="0" width="6.42914979757085"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="0" width="3.31983805668016"/>
     <col collapsed="false" hidden="false" max="23" min="22" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="9.85425101214575"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="9.96356275303644"/>
     <col collapsed="false" hidden="false" max="25" min="25" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="26" min="26" style="0" width="11.4615384615385"/>
     <col collapsed="false" hidden="false" max="27" min="27" style="0" width="9.21052631578947"/>
@@ -16045,8 +16052,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.4898785425101"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.8825910931174"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.3117408906883"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -16096,8 +16103,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.3522267206478"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -16147,10 +16154,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.7085020242915"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.6761133603239"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.31983805668016"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -16222,7 +16229,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.6761133603239"/>
     <col collapsed="false" hidden="false" max="973" min="5" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="974" style="0" width="5.1417004048583"/>
   </cols>
@@ -16429,18 +16436,18 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.39271255060729"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.2834008097166"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.39271255060729"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.6761133603239"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.96356275303644"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.0688259109312"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="12" min="10" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.3198380566802"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="30.6356275303644"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="30.8502024291498"/>
     <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -17502,9 +17509,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.17004048583"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.0688259109312"/>
     <col collapsed="false" hidden="false" max="997" min="5" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="998" style="0" width="5.1417004048583"/>
   </cols>
@@ -18979,10 +18986,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.246963562753"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6356275303644"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3198380566802"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.46153846153846"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
@@ -19132,9 +19139,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.1740890688259"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="29.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3846153846154"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="30.1012145748988"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -19353,11 +19360,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.6761133603239"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.85425101214575"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.5708502024291"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
@@ -24845,12 +24852,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.7085020242915"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.748987854251"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.9595141700405"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.8906882591093"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
@@ -25008,9 +25015,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.2834008097166"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1740890688259"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -25186,11 +25193,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6396761133603"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -25255,8 +25262,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.1012145748988"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.4615384615385"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
@@ -25421,10 +25428,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6761133603239"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.5991902834008"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.8137651821862"/>
     <col collapsed="false" hidden="false" max="6" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -25860,20 +25867,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5668016194332"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.2429149797571"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.46153846153846"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="11" min="10" style="0" width="11.1417004048583"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.4615384615385"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.85425101214575"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="18.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -26006,10 +26014,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1052631578947"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2105263157895"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -26199,12 +26207,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.4210526315789"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.7408906882591"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.8178137651822"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.21457489878543"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.85425101214575"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="22.6" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -26309,10 +26317,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.9595141700405"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.6396761133603"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49797570850202"/>
@@ -26320,9 +26328,9 @@
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.1417004048583"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="30.1012145748988"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="97.4777327935223"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="30.3157894736842"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="98.336032388664"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.85425101214575"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.45" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -26461,10 +26469,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.7085020242915"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.6761133603239"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.31983805668016"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -26539,8 +26547,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.0607287449393"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.3846153846154"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -26625,17 +26633,16 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3198380566802"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5708502024291"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4251012145749"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.53441295546559"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.85425101214575"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.85425101214575"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -26758,16 +26765,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.7813765182186"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="9.85425101214575"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.7813765182186"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.85425101214575"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.9" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -26888,9 +26895,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.9595141700405"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6396761133603"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.49797570850202"/>
@@ -26898,8 +26905,8 @@
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.1417004048583"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="30.1012145748988"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="30.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.85425101214575"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -27108,10 +27115,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.7085020242915"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.6761133603239"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.31983805668016"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -27186,9 +27193,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0323886639676"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -27264,8 +27271,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3157894736842"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.7813765182186"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -27344,10 +27351,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.5344129554656"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.4574898785425"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="40" width="8.24696356275304"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="40" width="12.1052631578947"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="40" width="12.2105263157895"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="40" width="6"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="40" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
@@ -27506,8 +27513,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.0688259109312"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.8178137651822"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
@@ -27904,10 +27911,10 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8502024291498"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.74898785425101"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.2105263157895"/>
     <col collapsed="false" hidden="false" max="1023" min="6" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="5.1417004048583"/>
   </cols>
@@ -28386,7 +28393,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.39271255060729"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="8" min="6" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.74898785425101"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.3886639676113"/>
@@ -29655,10 +29662,10 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.748987854251"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="6.85425101214575"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="41" width="9.4251012145749"/>
   </cols>
   <sheetData>
@@ -29832,12 +29839,12 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.24696356275304"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.5668016194332"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.21052631578947"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.2834008097166"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.6032388663968"/>
@@ -30289,14 +30296,14 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.96356275303644"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.0688259109312"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="12" min="9" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.0323886639676"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="26" min="16" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="27" min="27" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="8.57085020242915"/>

</xml_diff>

<commit_message>
CHanged default AR ID seq padding
</commit_message>
<xml_diff>
--- a/bika/lims/setupdata/test/test.xlsx
+++ b/bika/lims/setupdata/test/test.xlsx
@@ -275,7 +275,7 @@
     <t xml:space="preserve">Analysis Request</t>
   </si>
   <si>
-    <t xml:space="preserve">{sampleId}-R{seq:d}</t>
+    <t xml:space="preserve">{sampleId}-R{seq:02d}</t>
   </si>
   <si>
     <t xml:space="preserve">counter</t>
@@ -6133,7 +6133,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="99.834008097166"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="100.692307692308"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -6203,8 +6203,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -6254,8 +6254,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -6356,8 +6356,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="5" min="3" style="0" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -6696,14 +6696,14 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.21052631578947"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.53441295546559"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.85425101214575"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.1012145748988"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.0688259109312"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.96356275303644"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.60728744939271"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.0647773279352"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.2793522267206"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.31983805668016"/>
   </cols>
   <sheetData>
@@ -6881,10 +6881,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8542510121458"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="40" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="40" width="12.3198380566802"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="40" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="40" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="40" width="12.748987854251"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -7060,12 +7060,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.4574898785425"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.74898785425101"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -7286,8 +7286,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.1376518218623"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -7397,13 +7397,13 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.995951417004"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.74898785425101"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.74898785425101"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.60728744939271"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.7813765182186"/>
     <col collapsed="false" hidden="false" max="1023" min="9" style="0" width="6.74898785425101"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="5.78542510121457"/>
   </cols>
@@ -7833,10 +7833,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="18.2105263157895"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1018" min="9" style="0" width="8.57085020242915"/>
@@ -8128,8 +8128,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6032388663968"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1018" min="4" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1019" style="0" width="5.1417004048583"/>
@@ -8196,20 +8196,20 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="5" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="20.4615384615385"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="5" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="5" width="6.21457489878543"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="5" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="10.0688259109312"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="5" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -8558,11 +8558,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9595141700405"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="58.4858299595142"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="58.914979757085"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.7085020242915"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="86" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.5668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -8819,8 +8819,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.4615384615385"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -8961,9 +8961,9 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="10.0688259109312"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="21" min="6" style="0" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="21" min="6" style="0" width="10.1781376518219"/>
     <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -9191,7 +9191,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.5668016194332"/>
     <col collapsed="false" hidden="false" max="21" min="2" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.57085020242915"/>
   </cols>
@@ -9470,8 +9470,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.7773279352227"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="7.71255060728745"/>
   </cols>
   <sheetData>
@@ -9590,26 +9590,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.6761133603239"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.6720647773279"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.9959514170041"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="22.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -10761,18 +10761,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.4615384615385"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.3522267206478"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="34.7085020242915"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="33.5263157894737"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="39.9554655870445"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="34.919028340081"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="33.8502024291498"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="40.2753036437247"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="7.71255060728745"/>
   </cols>
   <sheetData>
@@ -10952,17 +10952,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1012145748988"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.7813765182186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.246963562753"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.0688259109312"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.3846153846154"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.8866396761134"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.6356275303644"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.1012145748988"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="37.17004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="7.71255060728745"/>
   </cols>
   <sheetData>
@@ -11137,9 +11137,9 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.8906882591093"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5708502024291"/>
   </cols>
@@ -11273,15 +11273,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8542510121458"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="31.0647773279352"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="7.71255060728745"/>
   </cols>
@@ -12143,8 +12143,8 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.3846153846154"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.5991902834008"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1012145748988"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.74898785425101"/>
   </cols>
   <sheetData>
@@ -12545,15 +12545,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.6761133603239"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.0647773279352"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8542510121457"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.71255060728745"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.9595141700405"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="5.35627530364372"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="7.71255060728745"/>
   </cols>
@@ -12772,15 +12772,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.4615384615385"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.8906882591093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.9959514170041"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.9230769230769"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.71255060728745"/>
   </cols>
   <sheetData>
@@ -12874,9 +12874,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.9919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.8502024291498"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.17004048583"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -12977,9 +12977,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.7813765182186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.6315789473684"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.2753036437247"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.0607287449393"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.5951417004049"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.31983805668016"/>
   </cols>
   <sheetData>
@@ -13115,7 +13115,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="25.7085020242915"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="3.31983805668016"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
@@ -13723,11 +13723,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="30.4210526315789"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.35627530364372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.2105263157895"/>
     <col collapsed="false" hidden="false" max="8" min="7" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.10526315789474"/>
@@ -13741,7 +13741,7 @@
     <col collapsed="false" hidden="false" max="20" min="20" style="0" width="6.42914979757085"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="0" width="3.31983805668016"/>
     <col collapsed="false" hidden="false" max="23" min="22" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="10.1781376518219"/>
     <col collapsed="false" hidden="false" max="25" min="25" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="26" min="26" style="0" width="11.4615384615385"/>
     <col collapsed="false" hidden="false" max="27" min="27" style="0" width="9.21052631578947"/>
@@ -16052,8 +16052,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.7408906882591"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.2429149797571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.165991902834"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -16103,8 +16103,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.7773279352227"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -16154,10 +16154,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.1376518218623"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8906882591093"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.31983805668016"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -16229,7 +16229,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8906882591093"/>
     <col collapsed="false" hidden="false" max="973" min="5" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="974" style="0" width="5.1417004048583"/>
   </cols>
@@ -16438,16 +16438,16 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.8906882591093"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.1781376518219"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="12" min="10" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.5344129554656"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="31.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -17509,9 +17509,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.4898785425101"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.7044534412955"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2834008097166"/>
     <col collapsed="false" hidden="false" max="997" min="5" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="998" style="0" width="5.1417004048583"/>
   </cols>
@@ -18986,10 +18986,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.4615384615385"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.0647773279352"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5344129554656"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.46153846153846"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
@@ -19139,9 +19139,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.4939271255061"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="30.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="30.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -19360,10 +19360,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.0688259109312"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.6720647773279"/>
     <col collapsed="false" hidden="false" max="7" min="5" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.5708502024291"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
@@ -24852,12 +24852,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.9230769230769"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9595141700405"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.1052631578947"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
@@ -25017,7 +25017,7 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -25193,11 +25193,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8542510121458"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.1740890688259"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -25262,8 +25262,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5303643724696"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.4615384615385"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
@@ -25428,10 +25428,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.0283400809717"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.2429149797571"/>
     <col collapsed="false" hidden="false" max="6" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -25867,20 +25867,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7813765182186"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.4574898785425"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.46153846153846"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="11" min="10" style="0" width="11.1417004048583"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.4615384615385"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.6761133603239"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="18.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -26013,10 +26014,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4251012145749"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -26206,11 +26207,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.0647773279352"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.3846153846154"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.8178137651822"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.21457489878543"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.67611336032389"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="22.6" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -26315,10 +26317,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8542510121457"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49797570850202"/>
@@ -26326,8 +26328,9 @@
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.1417004048583"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="30.5303643724696"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="99.1902834008097"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="30.7449392712551"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="100.048582995951"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.45" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -26466,10 +26469,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.1376518218623"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8906882591093"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.31983805668016"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -26544,8 +26547,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.7044534412955"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.0283400809717"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -26630,16 +26633,17 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5344129554656"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5708502024291"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.6396761133603"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.53441295546559"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -26762,14 +26766,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2105263157895"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.4615384615385"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.9" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -26890,9 +26896,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8542510121457"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.49797570850202"/>
@@ -26900,7 +26906,8 @@
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.1417004048583"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="30.5303643724696"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="30.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -27109,10 +27116,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.1376518218623"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8906882591093"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.31983805668016"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -27187,9 +27194,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -27265,8 +27272,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -27345,10 +27352,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.6720647773279"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="40" width="8.24696356275304"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="40" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="40" width="12.4251012145749"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="40" width="6"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="40" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
@@ -27507,8 +27514,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.2834008097166"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.8178137651822"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
@@ -27905,10 +27912,10 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.0647773279352"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.2793522267206"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.74898785425101"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.5303643724696"/>
     <col collapsed="false" hidden="false" max="1023" min="6" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="5.1417004048583"/>
   </cols>
@@ -29656,10 +29663,10 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9595141700405"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="6.85425101214575"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.4615384615385"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="41" width="9.4251012145749"/>
   </cols>
   <sheetData>
@@ -29833,9 +29840,9 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.24696356275304"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.7813765182186"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.21052631578947"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.3886639676113"/>
@@ -30290,14 +30297,14 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.96356275303644"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2834008097166"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="12" min="9" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.246963562753"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="26" min="16" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="27" min="27" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="8.57085020242915"/>

</xml_diff>

<commit_message>
Add UnitConversions and UnitConversion
</commit_message>
<xml_diff>
--- a/bika/lims/setupdata/test/test.xlsx
+++ b/bika/lims/setupdata/test/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="64"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -72,6 +72,7 @@
     <sheet name="Worksheet Template Layouts" sheetId="62" state="visible" r:id="rId63"/>
     <sheet name="Setup" sheetId="63" state="visible" r:id="rId64"/>
     <sheet name="Constants" sheetId="64" state="visible" r:id="rId65"/>
+    <sheet name="Unit Conversions" sheetId="65" state="visible" r:id="rId66"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -194,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3962" uniqueCount="1615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3983" uniqueCount="1629">
   <si>
     <t xml:space="preserve">Instructions</t>
   </si>
@@ -5039,6 +5040,48 @@
   </si>
   <si>
     <t xml:space="preserve">ZWL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">converted_unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">formula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit Conversions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit  Conversion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mg/L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value * 0.03 * 100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convert mg/L to a percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mg/g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value * 0.03 * 100 * 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convert mg/L to a mg/g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ºC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ºF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Value * 9 / 5) + 32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convert Celcius to Fahrenheit</t>
   </si>
 </sst>
 </file>
@@ -6154,12 +6197,12 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="1:1 A6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="104.226720647773"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="105.19028340081"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -6224,7 +6267,7 @@
   <dimension ref="1:10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O11" activeCellId="1" sqref="1:1 O11"/>
+      <selection pane="topLeft" activeCell="O11" activeCellId="0" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -6236,9 +6279,9 @@
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="12" min="9" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.8906882591093"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="24.1012145748988"/>
     <col collapsed="false" hidden="false" max="26" min="16" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="27" min="27" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="8.57085020242915"/>
@@ -6879,8 +6922,8 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -6948,13 +6991,13 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="1:1 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.4615384615385"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -6999,13 +7042,13 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O60" activeCellId="1" sqref="1:1 O60"/>
+      <selection pane="topLeft" activeCell="O60" activeCellId="0" sqref="O60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.4615384615385"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -7101,13 +7144,13 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I23" activeCellId="1" sqref="1:1 I23"/>
+      <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9595141700405"/>
     <col collapsed="false" hidden="false" max="5" min="3" style="0" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -7438,7 +7481,7 @@
   <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="1" sqref="1:1 B10"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -7446,14 +7489,14 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.21052631578947"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.53441295546559"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.85425101214575"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.1740890688259"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.96356275303644"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.60728744939271"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.9230769230769"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.31983805668016"/>
   </cols>
   <sheetData>
@@ -7626,15 +7669,15 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="40" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="40" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="40" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="40" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="40" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -7805,17 +7848,17 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="1" sqref="1:1 B9"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3157894736842"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.74898785425101"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -8031,13 +8074,13 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="1:1 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.6720647773279"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -8141,19 +8184,19 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="1:1 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.0647773279352"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.74898785425101"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.74898785425101"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.60728744939271"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.3198380566802"/>
     <col collapsed="false" hidden="false" max="1023" min="9" style="0" width="6.74898785425101"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="5.78542510121457"/>
   </cols>
@@ -8578,18 +8621,18 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="1" sqref="1:1 C8"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="5" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="20.995951417004"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="5" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="5" width="6.21457489878543"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="5" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="22.6032388663968"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="5" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="5" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="5" width="9.10526315789474"/>
@@ -8935,15 +8978,15 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="1:1 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.6761133603239"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="18.7449392712551"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1018" min="9" style="0" width="8.57085020242915"/>
@@ -9230,13 +9273,13 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="1:1 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1018" min="4" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1019" style="0" width="5.1417004048583"/>
@@ -9303,16 +9346,16 @@
   <dimension ref="1:14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="60.9514170040486"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="61.4858299595142"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.3522267206478"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="86" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.6356275303644"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -9564,13 +9607,13 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="1:1 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -9705,7 +9748,7 @@
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="1:1 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -9936,12 +9979,12 @@
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="1" sqref="1:1 A25"/>
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.5303643724696"/>
     <col collapsed="false" hidden="false" max="21" min="2" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.57085020242915"/>
   </cols>
@@ -10215,13 +10258,13 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="1:1 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6356275303644"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.8502024291498"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="7.71255060728745"/>
   </cols>
   <sheetData>
@@ -10335,31 +10378,31 @@
   <dimension ref="A1:W24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D37" activeCellId="1" sqref="1:1 D37"/>
+      <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.3157894736842"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.7449392712551"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.5668016194332"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="23.2429149797571"/>
     <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -11506,23 +11549,23 @@
   <dimension ref="A1:L65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="1" sqref="1:1 I6"/>
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.9230769230769"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="35.8866396761134"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="34.919028340081"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="41.5627530364373"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="36.2064777327935"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="35.1336032388664"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="41.8825910931174"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="7.71255060728745"/>
   </cols>
   <sheetData>
@@ -11697,22 +11740,22 @@
   <dimension ref="A1:K65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.7813765182186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8906882591093"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.2064777327935"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.3522267206478"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.0647773279352"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="38.2429149797571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.3846153846154"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="38.5627530364372"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="7.71255060728745"/>
   </cols>
   <sheetData>
@@ -11880,14 +11923,14 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="1" sqref="1:1 C13"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.4574898785425"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.6720647773279"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6396761133603"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.74898785425101"/>
   </cols>
   <sheetData>
@@ -12283,16 +12326,16 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="1" sqref="1:1 D28"/>
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5708502024291"/>
   </cols>
@@ -12421,20 +12464,20 @@
   <dimension ref="A1:K65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O26" activeCellId="1" sqref="1:1 O26"/>
+      <selection pane="topLeft" activeCell="O26" activeCellId="0" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.4615384615385"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.1012145748988"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.8866396761134"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="32.0283400809717"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="32.2429149797571"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="7.71255060728745"/>
   </cols>
@@ -13290,19 +13333,19 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="1" sqref="1:1 G4"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.8137651821862"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.71255060728745"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="5.35627530364372"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="7.71255060728745"/>
@@ -13517,20 +13560,20 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="1:1 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.995951417004"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.9595141700405"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="29.9919028340081"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.71255060728745"/>
   </cols>
   <sheetData>
@@ -13619,14 +13662,14 @@
   <dimension ref="1:6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="1:1 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.17004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.1336032388664"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.3481781376518"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="22.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -13722,14 +13765,14 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="1:1 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3157894736842"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.668016194332"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.2024291497976"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.0971659919028"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.6315789473684"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.31983805668016"/>
   </cols>
   <sheetData>
@@ -13860,12 +13903,12 @@
   <dimension ref="A1:F99"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="1" sqref="1:1 B18"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="26.3522267206478"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="3.31983805668016"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
@@ -14468,16 +14511,16 @@
   <dimension ref="A1:AE28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L33" activeCellId="1" sqref="1:1 L33"/>
+      <selection pane="topLeft" activeCell="L33" activeCellId="0" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="31.7085020242915"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.35627530364372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.7449392712551"/>
     <col collapsed="false" hidden="false" max="8" min="7" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.10526315789474"/>
@@ -16797,13 +16840,13 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.5263157894737"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.8502024291498"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.0971659919028"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -16848,13 +16891,13 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="1:1 B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6356275303644"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.8502024291498"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -16899,7 +16942,7 @@
   <dimension ref="A1:Y89"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="1" sqref="1:1 F20"/>
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -16907,16 +16950,16 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.39271255060729"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="12" min="10" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.0688259109312"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="32.5627530364372"/>
     <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -17973,15 +18016,15 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="1" sqref="1:1 B22"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.9919028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2064777327935"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.31983805668016"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -18045,7 +18088,7 @@
   <dimension ref="1:15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="1:1 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -18053,7 +18096,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="973" min="5" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="974" style="0" width="5.1417004048583"/>
   </cols>
@@ -18254,12 +18297,12 @@
   <dimension ref="1:103"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="1:1 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.8825910931174"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.2064777327935"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="997" min="5" style="0" width="8.57085020242915"/>
@@ -19731,15 +19774,15 @@
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="1" sqref="1:1 D9"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.1376518218623"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0688259109312"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.46153846153846"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
@@ -19884,14 +19927,14 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="1" sqref="1:1 A21"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="31.5991902834008"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="31.8137651821862"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -20105,15 +20148,15 @@
   <dimension ref="A1:I259"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M15" activeCellId="1" sqref="1:1 M15"/>
+      <selection pane="topLeft" activeCell="M15" activeCellId="0" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.2105263157895"/>
     <col collapsed="false" hidden="false" max="7" min="5" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.5708502024291"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
@@ -25597,17 +25640,17 @@
   <dimension ref="1:5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="1" sqref="1:1 C15"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.7813765182186"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
@@ -25760,7 +25803,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="1" sqref="1:1 B12"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -25938,16 +25981,15 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.8178137651822"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -26007,13 +26049,13 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="1:1 A5"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.4939271255061"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.4615384615385"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
@@ -26173,15 +26215,15 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E51" activeCellId="1" sqref="1:1 E51"/>
+      <selection pane="topLeft" activeCell="E51" activeCellId="0" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -26366,15 +26408,15 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="1:1 A11"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.1012145748988"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.4210526315789"/>
     <col collapsed="false" hidden="false" max="6" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.1376518218623"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -26805,19 +26847,19 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="1:1 B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3157894736842"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.3157894736842"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.46153846153846"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.9595141700405"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="11" min="10" style="0" width="11.1417004048583"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.4615384615385"/>
@@ -26952,12 +26994,12 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="1" sqref="1:1 A12"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.3481781376518"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.668016194332"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.8178137651822"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.21457489878543"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.46153846153846"/>
@@ -27062,15 +27104,15 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="1" sqref="1:1 A9"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.49797570850202"/>
@@ -27078,8 +27120,8 @@
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.1417004048583"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="31.8137651821862"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="103.692307692308"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="32.0283400809717"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="104.546558704453"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -27214,15 +27256,15 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="1" sqref="1:1 A21"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.9919028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2064777327935"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.31983805668016"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -27292,13 +27334,13 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="1:1 A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.3117408906883"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.6315789473684"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -27375,7 +27417,7 @@
   <dimension ref="1:3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="1" sqref="1:1 E4"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -27383,11 +27425,11 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0688259109312"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5708502024291"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.1740890688259"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.53441295546559"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.0323886639676"/>
@@ -27511,18 +27553,18 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="1:1 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.7449392712551"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="11" min="9" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.57085020242915"/>
@@ -27641,14 +27683,14 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="1" sqref="1:1 A12"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.49797570850202"/>
@@ -27656,7 +27698,7 @@
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.1417004048583"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="31.8137651821862"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="32.0283400809717"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -27861,15 +27903,15 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="1:1 B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.9919028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2064777327935"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.31983805668016"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -27939,15 +27981,15 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.7449392712551"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="40" width="8.24696356275304"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="40" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="40" width="12.9595141700405"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="40" width="6"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="40" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
@@ -28101,14 +28143,14 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="1:1 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6761133603239"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1740890688259"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -28179,13 +28221,13 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="1:1 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -28259,12 +28301,12 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3157894736842"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.8178137651822"/>
@@ -28656,16 +28698,16 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="1" sqref="1:1 D12"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.3522267206478"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.74898785425101"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.8137651821862"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.4939271255061"/>
     <col collapsed="false" hidden="false" max="1023" min="6" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="5.1417004048583"/>
   </cols>
@@ -29136,7 +29178,7 @@
   <dimension ref="A1:L200"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -30398,6 +30440,329 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="1:10"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3562753036437"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.7125506072875"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.7975708502024"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6761133603239"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="12" min="9" style="0" width="8.67611336032389"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="26" min="16" style="0" width="7.71255060728745"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="8.57085020242915"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="17" customFormat="true" ht="12.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1615</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>1616</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="AMI1" s="34"/>
+      <c r="AMJ1" s="34"/>
+    </row>
+    <row r="2" s="59" customFormat="true" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="28" t="s">
+        <v>1617</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="60"/>
+      <c r="S2" s="60"/>
+      <c r="T2" s="60"/>
+      <c r="U2" s="60"/>
+      <c r="V2" s="60"/>
+      <c r="W2" s="60"/>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="60"/>
+      <c r="Z2" s="60"/>
+      <c r="AMI2" s="61"/>
+      <c r="AMJ2" s="61"/>
+    </row>
+    <row r="3" s="17" customFormat="true" ht="12.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>1618</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>950</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="AMI3" s="34"/>
+      <c r="AMJ3" s="34"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="62" t="s">
+        <v>1619</v>
+      </c>
+      <c r="B4" s="62" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C4" s="62" t="s">
+        <v>1620</v>
+      </c>
+      <c r="D4" s="62" t="s">
+        <v>1621</v>
+      </c>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="63"/>
+      <c r="N4" s="65"/>
+      <c r="O4" s="64"/>
+      <c r="P4" s="66"/>
+      <c r="Q4" s="64"/>
+      <c r="R4" s="64"/>
+      <c r="S4" s="64"/>
+      <c r="T4" s="64"/>
+      <c r="U4" s="64"/>
+      <c r="V4" s="64"/>
+      <c r="W4" s="64"/>
+      <c r="X4" s="64"/>
+      <c r="Y4" s="64"/>
+      <c r="Z4" s="64"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="62" t="s">
+        <v>1619</v>
+      </c>
+      <c r="B5" s="62" t="s">
+        <v>1622</v>
+      </c>
+      <c r="C5" s="62" t="s">
+        <v>1623</v>
+      </c>
+      <c r="D5" s="62" t="s">
+        <v>1624</v>
+      </c>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="62"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="65"/>
+      <c r="O5" s="64"/>
+      <c r="P5" s="66"/>
+      <c r="Q5" s="64"/>
+      <c r="R5" s="64"/>
+      <c r="S5" s="64"/>
+      <c r="T5" s="64"/>
+      <c r="U5" s="64"/>
+      <c r="V5" s="64"/>
+      <c r="W5" s="64"/>
+      <c r="X5" s="64"/>
+      <c r="Y5" s="64"/>
+      <c r="Z5" s="64"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="62" t="s">
+        <v>1625</v>
+      </c>
+      <c r="B6" s="62" t="s">
+        <v>1626</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>1627</v>
+      </c>
+      <c r="D6" s="62" t="s">
+        <v>1628</v>
+      </c>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="63"/>
+      <c r="N6" s="65"/>
+      <c r="O6" s="64"/>
+      <c r="P6" s="66"/>
+      <c r="Q6" s="64"/>
+      <c r="R6" s="64"/>
+      <c r="S6" s="64"/>
+      <c r="T6" s="64"/>
+      <c r="U6" s="64"/>
+      <c r="V6" s="64"/>
+      <c r="W6" s="64"/>
+      <c r="X6" s="64"/>
+      <c r="Y6" s="64"/>
+      <c r="Z6" s="64"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="62"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="63"/>
+      <c r="N7" s="65"/>
+      <c r="O7" s="64"/>
+      <c r="P7" s="66"/>
+      <c r="Q7" s="64"/>
+      <c r="R7" s="64"/>
+      <c r="S7" s="64"/>
+      <c r="T7" s="64"/>
+      <c r="U7" s="64"/>
+      <c r="V7" s="64"/>
+      <c r="W7" s="64"/>
+      <c r="X7" s="64"/>
+      <c r="Y7" s="64"/>
+      <c r="Z7" s="64"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="62"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="63"/>
+      <c r="N8" s="65"/>
+      <c r="O8" s="64"/>
+      <c r="P8" s="66"/>
+      <c r="Q8" s="64"/>
+      <c r="R8" s="64"/>
+      <c r="S8" s="64"/>
+      <c r="T8" s="64"/>
+      <c r="U8" s="64"/>
+      <c r="V8" s="64"/>
+      <c r="W8" s="64"/>
+      <c r="X8" s="64"/>
+      <c r="Y8" s="64"/>
+      <c r="Z8" s="64"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="62"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="62"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="63"/>
+      <c r="N9" s="65"/>
+      <c r="O9" s="64"/>
+      <c r="P9" s="66"/>
+      <c r="Q9" s="64"/>
+      <c r="R9" s="64"/>
+      <c r="S9" s="64"/>
+      <c r="T9" s="64"/>
+      <c r="U9" s="64"/>
+      <c r="V9" s="64"/>
+      <c r="W9" s="64"/>
+      <c r="X9" s="64"/>
+      <c r="Y9" s="64"/>
+      <c r="Z9" s="64"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="62"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="64"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="62"/>
+      <c r="M10" s="63"/>
+      <c r="N10" s="65"/>
+      <c r="O10" s="64"/>
+      <c r="P10" s="66"/>
+      <c r="Q10" s="64"/>
+      <c r="R10" s="64"/>
+      <c r="S10" s="64"/>
+      <c r="T10" s="64"/>
+      <c r="U10" s="64"/>
+      <c r="V10" s="64"/>
+      <c r="W10" s="64"/>
+      <c r="X10" s="64"/>
+      <c r="Y10" s="64"/>
+      <c r="Z10" s="64"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="V2:Z2"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation allowBlank="true" error="Select an entry from the drop down list" errorTitle="Invalid entry" operator="equal" prompt="If the contact wants more than one publication method and the combination is not on the list, enter them by hand and separate with commas" promptTitle="Select valid publication preferences from the drop-down list" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="N4:N10" type="list">
+      <formula1>Constants!$H$2:$H$20</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" error="Select 0 or 1  from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 1 (True) or 0 (False) from the drop-down menu" promptTitle="Is  the contact permitted file attachments for emailed results?" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="P4:P10" type="list">
+      <formula1>Constants!$G$2:$G$3</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -30406,7 +30771,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H52" activeCellId="1" sqref="1:1 H52"/>
+      <selection pane="topLeft" activeCell="H52" activeCellId="0" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -30416,7 +30781,7 @@
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="6.85425101214575"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="41" width="9.4251012145749"/>
   </cols>
   <sheetData>
@@ -30582,7 +30947,7 @@
   <dimension ref="1:8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="1" sqref="1:1 H9"/>
+      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -30590,9 +30955,9 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.24696356275304"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8542510121457"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.3157894736842"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.21052631578947"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.3886639676113"/>
@@ -31039,7 +31404,7 @@
   <dimension ref="1:10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -31051,9 +31416,9 @@
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="12" min="9" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.8906882591093"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="24.1012145748988"/>
     <col collapsed="false" hidden="false" max="26" min="16" style="0" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="27" min="27" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="8.57085020242915"/>

</xml_diff>